<commit_message>
dawhar bolon talbain tohiruulgatai
</commit_message>
<xml_diff>
--- a/03_Analyz/result/filled_price_0626.xlsx
+++ b/03_Analyz/result/filled_price_0626.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Office\03_Analyz\result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BA21712-E55A-4A2A-B48A-53E70244FAB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79FF906F-0606-4F3C-9299-624FC65C00FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1948,13 +1948,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="S156" sqref="S156"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="7" max="7" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>